<commit_message>
Questions and Answers from Client
Text file outlining our questions for the client and the answers they
provided
</commit_message>
<xml_diff>
--- a/docs/ProgrammingLog.xlsx
+++ b/docs/ProgrammingLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\computing\Desktop\SEGroup4\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\computing\SEGroup4\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Spotify create playlist based on keywords</t>
+  </si>
+  <si>
+    <t>Navigating JSON structure of the return values</t>
+  </si>
+  <si>
+    <t>Printing out JSON and reading it</t>
   </si>
 </sst>
 </file>
@@ -119,7 +125,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,11 +152,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -173,25 +179,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -211,7 +202,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,7 +489,7 @@
   <dimension ref="C2:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,9 +606,13 @@
       <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="3"/>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>

</xml_diff>